<commit_message>
Arreglo de dependencias y fallos menores
</commit_message>
<xml_diff>
--- a/resultados/tabla_personalizada.xlsx
+++ b/resultados/tabla_personalizada.xlsx
@@ -689,7 +689,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>AMBOS SEXOS</t>
+          <t>Hombres</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>AMBOS SEXOS</t>
+          <t>Mujeres</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mejor distribución de comentarios y métodos
</commit_message>
<xml_diff>
--- a/resultados/tabla_personalizada.xlsx
+++ b/resultados/tabla_personalizada.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,339 +434,536 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sección</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Subsección</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Fila</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>E. Infantil - Primer ciclo</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>E. Infantil - Segundo ciclo</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>E. Primaria</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Educación Especial</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>ESO</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Bachillerato</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Bachillerato a distancia</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>CF Grado Básico</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>CF Grado Medio</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>CF Grado Medio a distancia</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Cursos de Especialización Grado Medio</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Cursos de Especialización Grado Medio a distancia</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>CF Grado Superior</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>CF Grado Superior a distancia</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Cursos de Especialización Grado Superior</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Cursos de Especialización Grado Superior a distancia</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Otros Programas Formativos</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Tabla</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Sección</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Subsección</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>TODOS LOS CENTROS</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AMBOS SEXOS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>01 ANDALUCÍA</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="D2" t="n">
         <v>1603826</v>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="n">
         <v>106619</v>
       </c>
-      <c r="D2" t="n">
+      <c r="F2" t="n">
         <v>221323</v>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
         <v>531221</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>9426</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>411932</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>125265</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>8537</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>14482</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
         <v>73480</v>
       </c>
-      <c r="L2" t="n">
+      <c r="N2" t="n">
         <v>3342</v>
       </c>
-      <c r="M2" t="n">
+      <c r="O2" t="n">
         <v>154</v>
       </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
         <v>79079</v>
       </c>
-      <c r="P2" t="n">
+      <c r="R2" t="n">
         <v>17575</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="S2" t="n">
         <v>888</v>
       </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
         <v>503</v>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>regimen_general</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>TODOS LOS CENTROS</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>AMBOS SEXOS</t>
-        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>TODOS LOS CENTROS</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AMBOS SEXOS</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>01 ANDALUCÍA</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="D3" t="n">
         <v>824964</v>
       </c>
-      <c r="C3" t="n">
+      <c r="E3" t="n">
         <v>55414</v>
       </c>
-      <c r="D3" t="n">
+      <c r="F3" t="n">
         <v>113556</v>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
         <v>273456</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>6306</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>212135</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>57897</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>4420</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>10370</v>
       </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
         <v>40959</v>
       </c>
-      <c r="L3" t="n">
+      <c r="N3" t="n">
         <v>1111</v>
       </c>
-      <c r="M3" t="n">
+      <c r="O3" t="n">
         <v>130</v>
       </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
         <v>40668</v>
       </c>
-      <c r="P3" t="n">
+      <c r="R3" t="n">
         <v>7511</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="S3" t="n">
         <v>712</v>
       </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
         <v>319</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>regimen_general</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>TODOS LOS CENTROS</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>Hombres</t>
-        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>TODOS LOS CENTROS</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AMBOS SEXOS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>01 ANDALUCÍA</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="D4" t="n">
         <v>778862</v>
       </c>
-      <c r="C4" t="n">
+      <c r="E4" t="n">
         <v>51205</v>
       </c>
-      <c r="D4" t="n">
+      <c r="F4" t="n">
         <v>107767</v>
       </c>
-      <c r="E4" t="n">
+      <c r="G4" t="n">
         <v>257765</v>
       </c>
-      <c r="F4" t="n">
+      <c r="H4" t="n">
         <v>3120</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>199797</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>67368</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>4117</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
         <v>4112</v>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
         <v>32521</v>
       </c>
-      <c r="L4" t="n">
+      <c r="N4" t="n">
         <v>2231</v>
       </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>24</v>
       </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
         <v>38411</v>
       </c>
-      <c r="P4" t="n">
+      <c r="R4" t="n">
         <v>10064</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="S4" t="n">
         <v>176</v>
       </c>
-      <c r="R4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
         <v>184</v>
       </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>regimen_general</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>TODOS LOS CENTROS</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AMBOS SEXOS</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1603826</v>
+      </c>
+      <c r="E5" t="n">
+        <v>106619</v>
+      </c>
+      <c r="F5" t="n">
+        <v>221323</v>
+      </c>
+      <c r="G5" t="n">
+        <v>531221</v>
+      </c>
+      <c r="H5" t="n">
+        <v>9426</v>
+      </c>
+      <c r="I5" t="n">
+        <v>411932</v>
+      </c>
+      <c r="J5" t="n">
+        <v>125265</v>
+      </c>
+      <c r="K5" t="n">
+        <v>8537</v>
+      </c>
+      <c r="L5" t="n">
+        <v>14482</v>
+      </c>
+      <c r="M5" t="n">
+        <v>73480</v>
+      </c>
+      <c r="N5" t="n">
+        <v>3342</v>
+      </c>
+      <c r="O5" t="n">
+        <v>154</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>79079</v>
+      </c>
+      <c r="R5" t="n">
+        <v>17575</v>
+      </c>
+      <c r="S5" t="n">
+        <v>888</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TODOS LOS CENTROS</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AMBOS SEXOS</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>824964</v>
+      </c>
+      <c r="E6" t="n">
+        <v>55414</v>
+      </c>
+      <c r="F6" t="n">
+        <v>113556</v>
+      </c>
+      <c r="G6" t="n">
+        <v>273456</v>
+      </c>
+      <c r="H6" t="n">
+        <v>6306</v>
+      </c>
+      <c r="I6" t="n">
+        <v>212135</v>
+      </c>
+      <c r="J6" t="n">
+        <v>57897</v>
+      </c>
+      <c r="K6" t="n">
+        <v>4420</v>
+      </c>
+      <c r="L6" t="n">
+        <v>10370</v>
+      </c>
+      <c r="M6" t="n">
+        <v>40959</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1111</v>
+      </c>
+      <c r="O6" t="n">
+        <v>130</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>40668</v>
+      </c>
+      <c r="R6" t="n">
+        <v>7511</v>
+      </c>
+      <c r="S6" t="n">
+        <v>712</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TODOS LOS CENTROS</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>AMBOS SEXOS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>778862</v>
+      </c>
+      <c r="E7" t="n">
+        <v>51205</v>
+      </c>
+      <c r="F7" t="n">
+        <v>107767</v>
+      </c>
+      <c r="G7" t="n">
+        <v>257765</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3120</v>
+      </c>
+      <c r="I7" t="n">
+        <v>199797</v>
+      </c>
+      <c r="J7" t="n">
+        <v>67368</v>
+      </c>
+      <c r="K7" t="n">
+        <v>4117</v>
+      </c>
+      <c r="L7" t="n">
+        <v>4112</v>
+      </c>
+      <c r="M7" t="n">
+        <v>32521</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2231</v>
+      </c>
+      <c r="O7" t="n">
+        <v>24</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>38411</v>
+      </c>
+      <c r="R7" t="n">
+        <v>10064</v>
+      </c>
+      <c r="S7" t="n">
+        <v>176</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>